<commit_message>
je sais pas ce qui a changer
</commit_message>
<xml_diff>
--- a/documents/hebergement +nomdedomaine.xlsx
+++ b/documents/hebergement +nomdedomaine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\WebApplication\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17702F54-ABC1-4ADF-BBD6-CB0FFB200A8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D51170-4E9C-4170-822B-20F367CD06E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92AA865A-05C8-4604-8D88-9B47BE41BB8D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>DEV1-S</t>
   </si>
@@ -100,6 +100,9 @@
   <si>
     <t>4,59 € HT
 (5,51 € TTC)</t>
+  </si>
+  <si>
+    <t>drim</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +130,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -188,9 +197,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,6 +204,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,7 +531,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,10 +543,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
@@ -549,7 +564,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
@@ -573,23 +588,23 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -601,15 +616,26 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="14">
+        <v>9.48</v>
+      </c>
+      <c r="D7" s="15">
+        <v>9.48</v>
       </c>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.3">
@@ -621,6 +647,7 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A4:A6"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>